<commit_message>
Different types of graphs
</commit_message>
<xml_diff>
--- a/project-2/results/spreadsheet/SingleCore_OpenMP.xlsx
+++ b/project-2/results/spreadsheet/SingleCore_OpenMP.xlsx
@@ -692,6 +692,13 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -710,13 +717,6 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -807,7 +807,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -906,11 +905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58548224"/>
-        <c:axId val="58554560"/>
+        <c:axId val="57499648"/>
+        <c:axId val="57505984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58548224"/>
+        <c:axId val="57499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -934,19 +933,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58554560"/>
+        <c:crossAx val="57505984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58554560"/>
+        <c:axId val="57505984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45"/>
@@ -970,14 +968,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58548224"/>
+        <c:crossAx val="57499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1041,12 +1038,27 @@
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:floor>
     <c:sideWall>
       <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
     </c:sideWall>
     <c:backWall>
       <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:backWall>
     <c:plotArea>
       <c:layout>
@@ -1824,12 +1836,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177556992"/>
-        <c:axId val="176472064"/>
-        <c:axId val="176372224"/>
+        <c:axId val="213208576"/>
+        <c:axId val="213172224"/>
+        <c:axId val="213072384"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="177556992"/>
+        <c:axId val="213208576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,7 +1877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176472064"/>
+        <c:crossAx val="213172224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1873,7 +1885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176472064"/>
+        <c:axId val="213172224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,12 +1922,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177556992"/>
+        <c:crossAx val="213208576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="176372224"/>
+        <c:axId val="213072384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,9 +1962,922 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176472064"/>
+        <c:crossAx val="213172224"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
+      <c:spPr>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>OpenMP on 1 computer</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> of 8 cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10389340348474747"/>
+          <c:y val="8.5681853824894502E-2"/>
+          <c:w val="0.8792187246617057"/>
+          <c:h val="0.77654242282327424"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.292435</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50765099999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1070500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3196400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8814500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.1624</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.160299999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.412100000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.26853399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50805199999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.12968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3397899999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9072500000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.1778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.159199999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$F$4:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.21863099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43643199999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94476400000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.89117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9556900000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1557399999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.9802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.098500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$G$4:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.20188300000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40808100000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87136800000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8266</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8927999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0802499999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.703600000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.433999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$H$4:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.17320199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40144800000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87283999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.85521</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1963499999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0692400000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.932099999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.872</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$I$4:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.208842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.436998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90896699999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0060600000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1491300000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5940100000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.4956</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.127400000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$J$4:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.207256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43353700000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91004700000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9154199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0070399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3247999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.101299999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.583300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$K$4:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.22620299999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43771500000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92542400000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9781500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0598599999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2142999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.908000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.2363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OpenMP!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OpenMP!$L$4:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.372807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43953399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99928600000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0243199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0821899999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4418699999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.3062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.768999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="243539968"/>
+        <c:axId val="170744576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="243539968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32"/>
+          <c:min val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Exponent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.50182597884646563"/>
+              <c:y val="0.92829961859837773"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="170744576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="170744576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.1235938185072419E-2"/>
+              <c:y val="0.37269053324428247"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243539968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2028,6 +2953,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2338,10 +3295,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -2349,16 +3306,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="7"/>
       <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +3450,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,48 +3462,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="6"/>
       <c r="D3" s="12" t="s">
         <v>7</v>
@@ -2598,7 +3555,7 @@
       <c r="G4" s="3">
         <v>0.20188300000000001</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="16">
         <v>0.17320199999999999</v>
       </c>
       <c r="I4" s="3">
@@ -2610,10 +3567,10 @@
       <c r="K4" s="3">
         <v>0.22620299999999999</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="20">
         <v>0.372807</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="23" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2630,7 +3587,7 @@
       <c r="D5" s="9">
         <v>0.50765099999999996</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="19">
         <v>0.50805199999999995</v>
       </c>
       <c r="F5" s="4">
@@ -2639,7 +3596,7 @@
       <c r="G5" s="4">
         <v>0.40808100000000003</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="15">
         <v>0.40144800000000003</v>
       </c>
       <c r="I5" s="4">
@@ -2654,7 +3611,7 @@
       <c r="L5" s="4">
         <v>0.43953399999999998</v>
       </c>
-      <c r="M5" s="17"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2669,13 +3626,13 @@
       <c r="D6" s="9">
         <v>1.1070500000000001</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="19">
         <v>1.12968</v>
       </c>
       <c r="F6" s="4">
         <v>0.94476400000000005</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="15">
         <v>0.87136800000000003</v>
       </c>
       <c r="H6" s="4">
@@ -2693,7 +3650,7 @@
       <c r="L6" s="4">
         <v>0.99928600000000001</v>
       </c>
-      <c r="M6" s="17"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2708,13 +3665,13 @@
       <c r="D7" s="9">
         <v>2.3196400000000001</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="19">
         <v>2.3397899999999998</v>
       </c>
       <c r="F7" s="4">
         <v>1.89117</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="15">
         <v>1.8266</v>
       </c>
       <c r="H7" s="4">
@@ -2732,7 +3689,7 @@
       <c r="L7" s="4">
         <v>2.0243199999999999</v>
       </c>
-      <c r="M7" s="17"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2747,13 +3704,13 @@
       <c r="D8" s="9">
         <v>4.8814500000000001</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="19">
         <v>4.9072500000000003</v>
       </c>
       <c r="F8" s="4">
         <v>3.9556900000000002</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="15">
         <v>3.8927999999999998</v>
       </c>
       <c r="H8" s="4">
@@ -2771,7 +3728,7 @@
       <c r="L8" s="4">
         <v>4.0821899999999998</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2786,7 +3743,7 @@
       <c r="D9" s="9">
         <v>10.1624</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="19">
         <v>10.1778</v>
       </c>
       <c r="F9" s="4">
@@ -2795,7 +3752,7 @@
       <c r="G9" s="4">
         <v>8.0802499999999995</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="15">
         <v>8.0692400000000006</v>
       </c>
       <c r="I9" s="4">
@@ -2810,7 +3767,7 @@
       <c r="L9" s="4">
         <v>8.4418699999999998</v>
       </c>
-      <c r="M9" s="17"/>
+      <c r="M9" s="24"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2825,13 +3782,13 @@
       <c r="D10" s="9">
         <v>21.160299999999999</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="19">
         <v>21.159199999999998</v>
       </c>
       <c r="F10" s="4">
         <v>16.9802</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="15">
         <v>16.703600000000002</v>
       </c>
       <c r="H10" s="4">
@@ -2849,7 +3806,7 @@
       <c r="L10" s="4">
         <v>17.3062</v>
       </c>
-      <c r="M10" s="17"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2864,16 +3821,16 @@
       <c r="D11" s="10">
         <v>43.412100000000002</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="18">
         <v>43.29</v>
       </c>
       <c r="F11" s="5">
         <v>35.098500000000001</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="14">
         <v>34.433999999999997</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="17">
         <v>34.872</v>
       </c>
       <c r="I11" s="5">
@@ -2888,7 +3845,7 @@
       <c r="L11" s="5">
         <v>35.768999999999998</v>
       </c>
-      <c r="M11" s="18"/>
+      <c r="M11" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>